<commit_message>
Debug: search->save source to source.xlsx->download
</commit_message>
<xml_diff>
--- a/data/source.xlsx
+++ b/data/source.xlsx
@@ -8,19 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PycharmWorkspace\Music-Download\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A760D597-252F-4B65-B0B8-23DEEBD5DD5E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F988E635-7E03-454E-A64B-32575760E04B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="music" sheetId="1" r:id="rId1"/>
+    <sheet name="log" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -345,8 +342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="A193" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -355,4 +352,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F866BA9F-3961-4176-93AE-E96B679FA961}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add & Update: README.md 添加使用介绍
</commit_message>
<xml_diff>
--- a/data/source.xlsx
+++ b/data/source.xlsx
@@ -1,46 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PycharmWorkspace\Music-Download\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F988E635-7E03-454E-A64B-32575760E04B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="music" sheetId="1" r:id="rId1"/>
-    <sheet name="log" sheetId="2" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="music" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="log" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
+  <si>
+    <t># COMMIT MUSIC_NAME SINGER_NAME SOURCE_LINK</t>
+  </si>
+  <si>
+    <t># COMMIT SOURCE SEARCH LOG</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -56,24 +57,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -88,44 +80,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -152,15 +144,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -187,7 +178,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -199,171 +189,231 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F866BA9F-3961-4176-93AE-E96B679FA961}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>